<commit_message>
Commit at end of sprint 1 / start of sprint 2
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -90,7 +90,22 @@
     <t>Local Log File Path</t>
   </si>
   <si>
-    <t>C:\Users\{0}\Desktop\Demo Robot Log_{1}.xlsx</t>
+    <t>Email Account</t>
+  </si>
+  <si>
+    <t>Process Log Path</t>
+  </si>
+  <si>
+    <t>C:\Users\Jsavory\Documents\GitHub\ea-annex-vii\Documents\Log\{0} Log</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\Annex_VII_Robot Log_{1}.xlsx</t>
+  </si>
+  <si>
+    <t>OCRF File Path</t>
+  </si>
+  <si>
+    <t>C:\Users\Jsavory\Documents\GitHub\ea-annex-vii\Documents\OCRF\{0}_Overseas Recovery facility database_IWE_V2.xlsx</t>
   </si>
 </sst>
 </file>
@@ -227,7 +242,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" name="Name" dataDxfId="5"/>
     <tableColumn id="2" name="Value" dataDxfId="4"/>
@@ -237,7 +252,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:B11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:B14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
     <tableColumn id="1" name="Name" dataDxfId="1"/>
     <tableColumn id="2" name="Value" dataDxfId="0"/>
@@ -543,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,49 +621,73 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>3</v>
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -663,10 +702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,12 +738,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -717,49 +756,71 @@
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B14" s="4">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest update from Dev to Live Support
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20550" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Orchestrator Folder Path</t>
   </si>
   <si>
-    <t>Email Completed Folder</t>
-  </si>
-  <si>
     <t>Email Exception Folder</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Inbox\Annex VII\Action Required</t>
   </si>
   <si>
-    <t>Inbox\Annex VII\Completed</t>
-  </si>
-  <si>
     <t>C:\Users\Jsavory\Documents\GitHub\ea-annex-vii\Documents\Attachments\</t>
   </si>
   <si>
@@ -96,23 +90,62 @@
     <t>Process Log Path</t>
   </si>
   <si>
-    <t>C:\Users\Jsavory\Documents\GitHub\ea-annex-vii\Documents\Log\{0} Log</t>
-  </si>
-  <si>
     <t>C:\Users\{0}\Desktop\Annex_VII_Robot Log_{1}.xlsx</t>
   </si>
   <si>
     <t>OCRF File Path</t>
   </si>
   <si>
-    <t>C:\Users\Jsavory\Documents\GitHub\ea-annex-vii\Documents\OCRF\20201006_Overseas Recovery facility database_IWE_V2.xlsx</t>
+    <t>Sharepoint URL</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Documents\OCRF\</t>
+  </si>
+  <si>
+    <t>OCRF Sharepoint Path</t>
+  </si>
+  <si>
+    <t>Annex VII Project/Robot Test Folder/20201006_Overseas Recovery facility database_IWE_V3.xlsx</t>
+  </si>
+  <si>
+    <t>Annex VII Project/Robot Test Folder/Master Sheets/{0}/{1} Log.xlsx</t>
+  </si>
+  <si>
+    <t>https://defra.sharepoint.com/teams/Team1952/</t>
+  </si>
+  <si>
+    <t>Process Log Sharepoint Path</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Documents\Log\</t>
+  </si>
+  <si>
+    <t>Breakpoint 2</t>
+  </si>
+  <si>
+    <t>Exception Recipient</t>
+  </si>
+  <si>
+    <t>jason.savory@environment-agency.gov.uk</t>
+  </si>
+  <si>
+    <t>Mail Save Path</t>
+  </si>
+  <si>
+    <t>Annex VII Project/Robot Test Folder/Correspondence/2019-21/Compulsory/{0}/</t>
+  </si>
+  <si>
+    <t>Email App Exception Folder</t>
+  </si>
+  <si>
+    <t>Inbox\Annex VII\Application Exceptions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +157,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,10 +187,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -169,8 +211,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -242,7 +288,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" name="Name" dataDxfId="5"/>
     <tableColumn id="2" name="Value" dataDxfId="4"/>
@@ -252,7 +298,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:B14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:B20" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
     <tableColumn id="1" name="Name" dataDxfId="1"/>
     <tableColumn id="2" name="Value" dataDxfId="0"/>
@@ -558,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,111 +630,159 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>7</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -702,10 +796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,111 +818,163 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4">
         <v>3</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
switched off pause points
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jsavory\Documents\GitHub\ea-annex-vii\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1006109\Downloads\ea-annex-vii\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1752CF-3159-4722-8211-E5FDD2AA55D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20550" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="10995" yWindow="-21915" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -144,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -288,20 +289,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" name="Value" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:B20" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B20" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="1"/>
-    <tableColumn id="2" name="Value" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,7 +604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -795,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +830,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -837,7 +838,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -968,8 +969,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
asset for adobe app location
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1006109\Downloads\ea-annex-vii\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\ea-annex-vii\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1752CF-3159-4722-8211-E5FDD2AA55D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018664E1-056C-4EC0-B301-66B788517352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10995" yWindow="-21915" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="30" windowWidth="20460" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Inbox\Annex VII\Application Exceptions</t>
+  </si>
+  <si>
+    <t>Adobe File Path</t>
+  </si>
+  <si>
+    <t>C:\Program Files\Adobe\Reader 11.0\Reader\AcroRd32.exe</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="4"/>
@@ -299,7 +305,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B20" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="A1:B21" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value" dataDxfId="0"/>
@@ -605,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,105 +690,113 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -797,10 +811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,112 +879,120 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B21" s="4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>